<commit_message>
Changed Config file, variable "scope"
</commit_message>
<xml_diff>
--- a/connector/InputFormat.xlsx
+++ b/connector/InputFormat.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SBTi\connector\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="47925" windowHeight="17835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="47925" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="Company data" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>Target_classification</t>
   </si>
   <si>
-    <t>Scope</t>
-  </si>
-  <si>
     <t>coverage</t>
   </si>
   <si>
@@ -197,14 +194,17 @@
   </si>
   <si>
     <t>reduction_ambition</t>
+  </si>
+  <si>
+    <t>scope</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -250,7 +250,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -259,6 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -268,7 +269,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -327,7 +327,7 @@
     <tableColumn id="1" name="company_name"/>
     <tableColumn id="2" name="company_ID"/>
     <tableColumn id="3" name="Target_classification"/>
-    <tableColumn id="4" name="Scope"/>
+    <tableColumn id="4" name="scope"/>
     <tableColumn id="5" name="coverage"/>
     <tableColumn id="6" name="reduction_ambition"/>
     <tableColumn id="7" name="base_year"/>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,32 +636,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="6" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -721,10 +721,10 @@
         <v>1123</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3">
         <v>15943</v>
@@ -756,10 +756,10 @@
         <v>4231</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -767,59 +767,59 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +842,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,20 +858,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>17</v>
@@ -894,22 +894,22 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
         <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" t="s">
-        <v>26</v>
       </c>
       <c r="J2" t="s">
         <v>16</v>
@@ -923,10 +923,10 @@
         <v>1123</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -952,10 +952,10 @@
         <v>1123</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -981,7 +981,7 @@
         <v>1123</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5">
         <v>0.6</v>
@@ -1007,10 +1007,10 @@
         <v>1123</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6">
         <v>0.5</v>
@@ -1038,65 +1038,65 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1115,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
@@ -1128,13 +1128,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
       <c r="B2">
         <v>1123</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="4">
         <v>123.456</v>
       </c>
     </row>
@@ -1155,7 +1155,7 @@
       <c r="B3">
         <v>4231</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>582.41890000000001</v>
       </c>
     </row>
@@ -1164,56 +1164,56 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="7">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="7">
+        <v>40</v>
+      </c>
+      <c r="C5" s="4">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrated data_provider_input and target_valuation_protocol within the API
As well as correct the target_valuation_protocol hardcoded column names
</commit_message>
<xml_diff>
--- a/connector/InputFormat.xlsx
+++ b/connector/InputFormat.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Target data" sheetId="2" r:id="rId2"/>
     <sheet name="User input" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
   <si>
     <t>company_name</t>
   </si>
   <si>
-    <t>company_ID</t>
-  </si>
-  <si>
     <t>GHG_scope12</t>
   </si>
   <si>
@@ -112,12 +109,6 @@
     <t>Optional (assume equal to base if not available)</t>
   </si>
   <si>
-    <t>Company_name</t>
-  </si>
-  <si>
-    <t>Company_ID</t>
-  </si>
-  <si>
     <t>Allocation</t>
   </si>
   <si>
@@ -197,6 +188,33 @@
   </si>
   <si>
     <t>scope</t>
+  </si>
+  <si>
+    <t>company_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abs 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Int 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Int 2</t>
+  </si>
+  <si>
+    <t>target_reference_number</t>
+  </si>
+  <si>
+    <t>% emissions in Scope</t>
+  </si>
+  <si>
+    <t>% achieved (emissions)</t>
+  </si>
+  <si>
+    <t>target_year</t>
+  </si>
+  <si>
+    <t>% reduction from base year</t>
   </si>
 </sst>
 </file>
@@ -206,7 +224,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,13 +239,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -252,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -260,6 +310,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -300,7 +361,7 @@
   <autoFilter ref="A2:P42"/>
   <tableColumns count="16">
     <tableColumn id="1" name="company_name"/>
-    <tableColumn id="2" name="company_ID"/>
+    <tableColumn id="2" name="company_id"/>
     <tableColumn id="3" name="CDP_ACS_industry"/>
     <tableColumn id="4" name="country"/>
     <tableColumn id="5" name="industry"/>
@@ -321,11 +382,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:J30" totalsRowShown="0">
-  <autoFilter ref="A2:J30"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A2:O30" totalsRowShown="0">
+  <autoFilter ref="A2:O30"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="company_name"/>
-    <tableColumn id="2" name="company_ID"/>
+    <tableColumn id="2" name="company_id"/>
     <tableColumn id="3" name="Target_classification"/>
     <tableColumn id="4" name="scope"/>
     <tableColumn id="5" name="coverage"/>
@@ -334,6 +395,11 @@
     <tableColumn id="8" name="end_year"/>
     <tableColumn id="9" name="start_year"/>
     <tableColumn id="10" name="SBTi_status"/>
+    <tableColumn id="11" name="target_reference_number"/>
+    <tableColumn id="12" name="% reduction from base year"/>
+    <tableColumn id="13" name="% emissions in Scope"/>
+    <tableColumn id="14" name="% achieved (emissions)"/>
+    <tableColumn id="15" name="target_year"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -343,8 +409,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:C23" totalsRowShown="0">
   <autoFilter ref="A1:C23"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Company_name"/>
-    <tableColumn id="2" name="Company_ID"/>
+    <tableColumn id="1" name="company_name"/>
+    <tableColumn id="2" name="company_id"/>
     <tableColumn id="3" name="Allocation"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -617,7 +683,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,95 +702,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="5" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
       <c r="N2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
         <v>18</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1123</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G3">
         <v>15943</v>
@@ -750,76 +816,76 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>4231</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +908,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,26 +921,27 @@
     <col min="8" max="8" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="21" customWidth="1"/>
     <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -883,50 +950,65 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1123</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -943,19 +1025,34 @@
       <c r="I3">
         <v>2020</v>
       </c>
+      <c r="K3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="6">
+        <v>29</v>
+      </c>
+      <c r="M3" s="6">
+        <v>100</v>
+      </c>
+      <c r="N3" s="6">
+        <v>100</v>
+      </c>
+      <c r="O3" s="6">
+        <v>2020</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>1123</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -972,16 +1069,31 @@
       <c r="I4">
         <v>2019</v>
       </c>
+      <c r="K4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="6">
+        <v>30</v>
+      </c>
+      <c r="M4" s="6">
+        <v>100</v>
+      </c>
+      <c r="N4" s="6">
+        <v>58</v>
+      </c>
+      <c r="O4" s="6">
+        <v>2020</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>1123</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5">
         <v>0.6</v>
@@ -998,19 +1110,34 @@
       <c r="I5">
         <v>2018</v>
       </c>
+      <c r="K5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="6">
+        <v>40</v>
+      </c>
+      <c r="M5" s="6">
+        <v>93</v>
+      </c>
+      <c r="N5" s="6">
+        <v>89</v>
+      </c>
+      <c r="O5" s="6">
+        <v>2020</v>
+      </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>1123</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <v>0.5</v>
@@ -1024,10 +1151,17 @@
       <c r="I6">
         <v>2020</v>
       </c>
+      <c r="K6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>4231</v>
@@ -1035,68 +1169,171 @@
       <c r="E7">
         <v>0.67</v>
       </c>
+      <c r="K7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="6">
+        <v>70</v>
+      </c>
+      <c r="M7" s="6">
+        <v>100</v>
+      </c>
+      <c r="N7" s="6">
+        <v>27</v>
+      </c>
+      <c r="O7" s="6">
+        <v>2025</v>
+      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="6">
+        <v>20</v>
+      </c>
+      <c r="M8" s="6">
+        <v>82</v>
+      </c>
+      <c r="N8" s="6">
+        <v>100</v>
+      </c>
+      <c r="O8" s="6">
+        <v>2020</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="6">
+        <v>100</v>
+      </c>
+      <c r="M9" s="6">
+        <v>94</v>
+      </c>
+      <c r="N9" s="6">
+        <v>24</v>
+      </c>
+      <c r="O9" s="6">
+        <v>2050</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="6">
+        <v>25</v>
+      </c>
+      <c r="M10" s="6">
+        <v>100</v>
+      </c>
+      <c r="N10" s="6">
+        <v>90</v>
+      </c>
+      <c r="O10" s="6">
+        <v>2020</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="6">
+        <v>20</v>
+      </c>
+      <c r="M11" s="6">
+        <v>100</v>
+      </c>
+      <c r="N11" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="O11">
+        <v>2020</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" s="6">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12">
+        <v>2020</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" s="6">
+        <v>20</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13" s="6">
+        <v>95</v>
+      </c>
+      <c r="O13">
+        <v>2020</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1105,8 +1342,9 @@
     <mergeCell ref="D1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1116,7 +1354,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,18 +1366,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>1123</v>
@@ -1150,7 +1388,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>4231</v>
@@ -1161,10 +1399,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4">
         <v>200</v>
@@ -1172,10 +1410,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4">
         <v>1000</v>
@@ -1183,37 +1421,37 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>